<commit_message>
added toggle to manage_patients tab
</commit_message>
<xml_diff>
--- a/patient_data/Max_78267819/patient_ml_data.xlsx
+++ b/patient_data/Max_78267819/patient_ml_data.xlsx
@@ -22,13 +22,13 @@
     <t>Intestinal Signs</t>
   </si>
   <si>
-    <t>Depression, Lethargy</t>
+    <t>Depression</t>
   </si>
   <si>
     <t>Dyspnea</t>
   </si>
   <si>
-    <t/>
+    <t>Tenesmus</t>
   </si>
 </sst>
 </file>

</xml_diff>